<commit_message>
add images from ENT
</commit_message>
<xml_diff>
--- a/Planning Prévisionnel.xlsx
+++ b/Planning Prévisionnel.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="11_690482DC28E5EB85B98D7722DFE2FD8A16B8664E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20D7E3B9-8A8C-4454-8706-8C9E356BE10A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -72,9 +73,6 @@
     <t>Plan du Projet</t>
   </si>
   <si>
-    <t>Designs des Persos</t>
-  </si>
-  <si>
     <t>Création des Classes</t>
   </si>
   <si>
@@ -97,12 +95,15 @@
   </si>
   <si>
     <t xml:space="preserve">    Numéros des semaines basés sur le calendrier pédagogique</t>
+  </si>
+  <si>
+    <t>Récolte des images</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -158,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -178,10 +179,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,11 +461,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,38 +521,45 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C4" s="4"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="3"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="3"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -564,8 +571,9 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -577,9 +585,8 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="10"/>
+        <v>21</v>
+      </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -592,13 +599,13 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L10" s="3"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L11" s="3"/>
     </row>
@@ -615,7 +622,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>

</xml_diff>